<commit_message>
Updated with changes requested by Customer Success team
</commit_message>
<xml_diff>
--- a/Contoso - Sales - Current Release/Dataverse Data/3 🏭 Accounts for Import.xlsx
+++ b/Contoso - Sales - Current Release/Dataverse Data/3 🏭 Accounts for Import.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/misewell_microsoft_com/Documents/Documents/GitHub/ContosoBI/Contoso - Sales - Current Release/Dataverse Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_ADF37D841EA345F0FA330A5DCFB5940FC38FE545" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81310E73-FCD4-430F-A9DC-86474532F34B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_ADF37D841EA345F0FA330A5DCFB5940FC38FE545" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDE90331-5881-40AC-B388-9019E3F6007C}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-2610" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45465" yWindow="-945" windowWidth="34050" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Accounts - For Import" sheetId="1" r:id="rId1"/>
     <sheet name="hiddenSheet" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="238">
   <si>
     <t>(Do Not Modify) Account</t>
   </si>
@@ -691,6 +688,66 @@
   </si>
   <si>
     <t>Bridgewater</t>
+  </si>
+  <si>
+    <t>Allie Bellew</t>
+  </si>
+  <si>
+    <t>Karen Berg</t>
+  </si>
+  <si>
+    <t>David So</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Amy Alberts</t>
+  </si>
+  <si>
+    <t>Eric Gruber</t>
+  </si>
+  <si>
+    <t>Kelly Krout</t>
+  </si>
+  <si>
+    <t>Christa Geller</t>
+  </si>
+  <si>
+    <t>Anne Weiler</t>
+  </si>
+  <si>
+    <t>Greg Winston</t>
+  </si>
+  <si>
+    <t>Alan Steiner</t>
+  </si>
+  <si>
+    <t>Jeff Hay</t>
+  </si>
+  <si>
+    <t>Carlos Grilo</t>
+  </si>
+  <si>
+    <t>Jamie Reding</t>
+  </si>
+  <si>
+    <t>Sanjay Shah</t>
+  </si>
+  <si>
+    <t>Alicia Thomber</t>
+  </si>
+  <si>
+    <t>Sven Mortensen</t>
+  </si>
+  <si>
+    <t>Molly Clark</t>
+  </si>
+  <si>
+    <t>Renee Lo</t>
+  </si>
+  <si>
+    <t>Spencer Low</t>
   </si>
 </sst>
 </file>
@@ -844,47 +901,12 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Import Date"/>
-      <sheetName val="Accounts"/>
-      <sheetName val="Products"/>
-      <sheetName val="Cases"/>
-      <sheetName val="Cases - Import Format"/>
-      <sheetName val="Opportunities"/>
-      <sheetName val="Opportunities - Import Format"/>
-      <sheetName val="Territories"/>
-      <sheetName val="Owners"/>
-      <sheetName val="Industries"/>
-      <sheetName val="Marketing Campaigns"/>
-      <sheetName val="Contacts"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J81" totalsRowShown="0">
   <autoFilter ref="A1:J81" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J81">
+    <sortCondition ref="D1:D81"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Account"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
@@ -894,21 +916,17 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Address 1: State/Province" dataDxfId="2" dataCellStyle="Normal"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Address 1: Country/Region" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Territory" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Industry" dataCellStyle="Normal">
-      <calculatedColumnFormula>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Owner" dataCellStyle="Normal">
-      <calculatedColumnFormula>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Industry" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Owner" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -946,7 +964,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1052,7 +1070,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1194,7 +1212,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1206,10 +1224,10 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:J81"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
@@ -1220,7 +1238,7 @@
     <col min="10" max="10" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1252,233 +1270,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Brokers</v>
-      </c>
-      <c r="J2" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Allie Bellew</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+        <v>85</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Legal Services</v>
-      </c>
-      <c r="J3" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Karen Berg</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4" s="3" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Durable Manufacturing</v>
-      </c>
-      <c r="J4" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>David So</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5"/>
       <c r="C5"/>
-      <c r="D5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v/>
-      </c>
-      <c r="J5" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Amy Alberts</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6" s="3" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Equipment Rental and Leasing</v>
-      </c>
-      <c r="J6" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Eric Gruber</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Eating and Drinking Places</v>
-      </c>
-      <c r="J7" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>David So</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Agriculture and Non-petrol Natural Resource Extraction</v>
-      </c>
-      <c r="J8" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Kelly Krout</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Equipment Rental and Leasing</v>
-      </c>
-      <c r="J9" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Christa Geller</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>10</v>
@@ -1486,107 +1488,99 @@
       <c r="H10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I10" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Agriculture and Non-petrol Natural Resource Extraction</v>
-      </c>
-      <c r="J10" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Amy Alberts</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Eating and Drinking Places</v>
-      </c>
-      <c r="J11" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I11" t="s">
+        <v>221</v>
+      </c>
+      <c r="J11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12" s="3" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Consulting</v>
-      </c>
-      <c r="J12" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Amy Alberts</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" s="4" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Business Services</v>
-      </c>
-      <c r="J13" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Allie Bellew</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14"/>
       <c r="C14"/>
-      <c r="D14" s="3" t="s">
-        <v>90</v>
+      <c r="D14" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>10</v>
@@ -1594,404 +1588,374 @@
       <c r="H14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I14" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Broadcasting Printing and Publishing</v>
-      </c>
-      <c r="J14" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Kelly Krout</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I14" t="s">
+        <v>221</v>
+      </c>
+      <c r="J14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Insurance</v>
-      </c>
-      <c r="J15" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Karen Berg</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" s="3" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Financial</v>
-      </c>
-      <c r="J16" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Greg Winston</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17" s="4" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Accounting</v>
-      </c>
-      <c r="J17" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Amy Alberts</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" s="3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Inbound Repair and Services</v>
-      </c>
-      <c r="J18" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Eric Gruber</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19" s="4" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alan Steiner</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="4" t="s">
+      <c r="D20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I20" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Distributors, Dispatchers and Processors</v>
-      </c>
-      <c r="J20" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21" s="4" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Brokers</v>
-      </c>
-      <c r="J21" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Amy Alberts</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="4" t="s">
+      <c r="D22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I22" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Building Supply Retail</v>
-      </c>
-      <c r="J22" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Kelly Krout</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Equipment Rental and Leasing</v>
-      </c>
-      <c r="J23" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Christa Geller</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I24" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Food and Tobacco Processing</v>
-      </c>
-      <c r="J24" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jeff Hay</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I25" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Accounting</v>
-      </c>
-      <c r="J25" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alan Steiner</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I26" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Inbound Capital Intensive Processing</v>
-      </c>
-      <c r="J26" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jeff Hay</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Design, Direction and Creative Management</v>
-      </c>
-      <c r="J27" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Carlos Grilo</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28" s="3" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>126</v>
+        <v>12</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Financial</v>
-      </c>
-      <c r="J28" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Eric Gruber</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="I28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>10</v>
@@ -1999,80 +1963,74 @@
       <c r="H29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I29" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Food and Tobacco Processing</v>
-      </c>
-      <c r="J29" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Eric Gruber</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I29" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30" s="3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I30" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Doctor's Offices and Clinics</v>
-      </c>
-      <c r="J30" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I30" t="s">
+        <v>221</v>
+      </c>
+      <c r="J30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31" s="4" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I31" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Consumer Services</v>
-      </c>
-      <c r="J31" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32" s="3" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>10</v>
@@ -2080,26 +2038,24 @@
       <c r="H32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I32" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Entertainment Retail</v>
-      </c>
-      <c r="J32" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Christa Geller</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I32" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33" s="4" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>10</v>
@@ -2107,26 +2063,24 @@
       <c r="H33" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I33" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Non-Durable Merchandise Retail</v>
-      </c>
-      <c r="J33" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jamie Reding</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I33" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34" s="3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>10</v>
@@ -2134,50 +2088,46 @@
       <c r="H34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I34" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v/>
-      </c>
-      <c r="J34" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jamie Reding</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35" s="4" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I35" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Inbound Capital Intensive Processing</v>
-      </c>
-      <c r="J35" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Eric Gruber</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+      <c r="I35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>143</v>
@@ -2188,26 +2138,24 @@
       <c r="H36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I36" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Insurance</v>
-      </c>
-      <c r="J36" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Sanjay Shah</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I36" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37" s="4" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>10</v>
@@ -2215,134 +2163,124 @@
       <c r="H37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I37" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Entertainment Retail</v>
-      </c>
-      <c r="J37" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>David So</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I37" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Doctor's Offices and Clinics</v>
-      </c>
-      <c r="J38" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Carlos Grilo</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+      <c r="I38" t="s">
+        <v>38</v>
+      </c>
+      <c r="J38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39"/>
       <c r="C39"/>
-      <c r="D39" s="4" t="s">
-        <v>148</v>
+      <c r="D39" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I39" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Agriculture and Non-petrol Natural Resource Extraction</v>
-      </c>
-      <c r="J39" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alan Steiner</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+      <c r="I39" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I40" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Insurance</v>
-      </c>
-      <c r="J40" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Sanjay Shah</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+      <c r="I40" t="s">
+        <v>47</v>
+      </c>
+      <c r="J40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I41" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Insurance</v>
-      </c>
-      <c r="J41" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jamie Reding</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="I41" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>10</v>
@@ -2350,286 +2288,264 @@
       <c r="H42" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I42" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Durable Manufacturing</v>
-      </c>
-      <c r="J42" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I42" t="s">
+        <v>32</v>
+      </c>
+      <c r="J42" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43"/>
       <c r="C43"/>
-      <c r="D43" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I43" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Non-Durable Merchandise Retail</v>
-      </c>
-      <c r="J43" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I43" t="s">
+        <v>41</v>
+      </c>
+      <c r="J43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44"/>
       <c r="C44"/>
-      <c r="D44" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I44" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Legal Services</v>
-      </c>
-      <c r="J44" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Sven Mortensen</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45"/>
       <c r="C45"/>
-      <c r="D45" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I45" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Building Supply Retail</v>
-      </c>
-      <c r="J45" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Allie Bellew</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D45" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46"/>
       <c r="C46"/>
-      <c r="D46" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I46" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Non-Durable Merchandise Retail</v>
-      </c>
-      <c r="J46" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Sven Mortensen</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D46" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I46" t="s">
+        <v>30</v>
+      </c>
+      <c r="J46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47"/>
       <c r="C47"/>
-      <c r="D47" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I47" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Broadcasting Printing and Publishing</v>
-      </c>
-      <c r="J47" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alan Steiner</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D47" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48"/>
       <c r="C48"/>
-      <c r="D48" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I48" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Broadcasting Printing and Publishing</v>
-      </c>
-      <c r="J48" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Amy Alberts</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J48" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49"/>
       <c r="C49"/>
-      <c r="D49" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I49" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Legal Services</v>
-      </c>
-      <c r="J49" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Molly Clark</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D49" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B50"/>
       <c r="C50"/>
-      <c r="D50" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F50" s="4" t="s">
+      <c r="D50" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="4" t="s">
+      <c r="G50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I50" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Brokers</v>
-      </c>
-      <c r="J50" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Kelly Krout</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I50" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B51"/>
       <c r="C51"/>
-      <c r="D51" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I51" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Business Services</v>
-      </c>
-      <c r="J51" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Renee Lo</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="D51" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" t="s">
+        <v>22</v>
+      </c>
+      <c r="J51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I52" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Food and Tobacco Processing</v>
-      </c>
-      <c r="J52" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.4">
+        <v>82</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I52" t="s">
+        <v>39</v>
+      </c>
+      <c r="J52" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53" s="4" t="s">
@@ -2647,16 +2563,14 @@
       <c r="H53" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I53" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Financial</v>
-      </c>
-      <c r="J53" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Christa Geller</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I53" t="s">
+        <v>42</v>
+      </c>
+      <c r="J53" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54" s="3" t="s">
@@ -2674,16 +2588,14 @@
       <c r="H54" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I54" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Business Services</v>
-      </c>
-      <c r="J54" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Allie Bellew</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55" s="4" t="s">
@@ -2701,16 +2613,14 @@
       <c r="H55" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I55" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Distributors, Dispatchers and Processors</v>
-      </c>
-      <c r="J55" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Carlos Grilo</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I55" t="s">
+        <v>36</v>
+      </c>
+      <c r="J55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56" s="3" t="s">
@@ -2728,16 +2638,14 @@
       <c r="H56" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I56" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Legal Services</v>
-      </c>
-      <c r="J56" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I56" t="s">
+        <v>46</v>
+      </c>
+      <c r="J56" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57" s="4" t="s">
@@ -2755,16 +2663,14 @@
       <c r="H57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I57" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Design, Direction and Creative Management</v>
-      </c>
-      <c r="J57" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I57" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58" s="3" t="s">
@@ -2782,16 +2688,14 @@
       <c r="H58" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I58" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Consulting</v>
-      </c>
-      <c r="J58" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Renee Lo</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59" s="4" t="s">
@@ -2809,16 +2713,14 @@
       <c r="H59" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I59" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Outbound Consumer Service</v>
-      </c>
-      <c r="J59" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Sven Mortensen</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I59" t="s">
+        <v>48</v>
+      </c>
+      <c r="J59" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60" s="3" t="s">
@@ -2836,16 +2738,14 @@
       <c r="H60" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I60" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Doctor's Offices and Clinics</v>
-      </c>
-      <c r="J60" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Spencer Low</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I60" t="s">
+        <v>37</v>
+      </c>
+      <c r="J60" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61" s="4" t="s">
@@ -2863,16 +2763,14 @@
       <c r="H61" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I61" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Inbound Capital Intensive Processing</v>
-      </c>
-      <c r="J61" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I61" t="s">
+        <v>43</v>
+      </c>
+      <c r="J61" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62" s="3" t="s">
@@ -2890,16 +2788,14 @@
       <c r="H62" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I62" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Entertainment Retail</v>
-      </c>
-      <c r="J62" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Christa Geller</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I62" t="s">
+        <v>40</v>
+      </c>
+      <c r="J62" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63" s="4" t="s">
@@ -2917,16 +2813,14 @@
       <c r="H63" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I63" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Non-Durable Merchandise Retail</v>
-      </c>
-      <c r="J63" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Molly Clark</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I63" t="s">
+        <v>47</v>
+      </c>
+      <c r="J63" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64" s="3" t="s">
@@ -2944,16 +2838,14 @@
       <c r="H64" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I64" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Consumer Services</v>
-      </c>
-      <c r="J64" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Renee Lo</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I64" t="s">
+        <v>34</v>
+      </c>
+      <c r="J64" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65" s="4" t="s">
@@ -2971,16 +2863,14 @@
       <c r="H65" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I65" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Outbound Consumer Service</v>
-      </c>
-      <c r="J65" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Molly Clark</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I65" t="s">
+        <v>48</v>
+      </c>
+      <c r="J65" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66" s="3" t="s">
@@ -2998,16 +2888,14 @@
       <c r="H66" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I66" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Inbound Repair and Services</v>
-      </c>
-      <c r="J66" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jeff Hay</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I66" t="s">
+        <v>44</v>
+      </c>
+      <c r="J66" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67" s="4" t="s">
@@ -3025,16 +2913,14 @@
       <c r="H67" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I67" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Legal Services</v>
-      </c>
-      <c r="J67" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jamie Reding</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I67" t="s">
+        <v>46</v>
+      </c>
+      <c r="J67" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68" s="3" t="s">
@@ -3052,16 +2938,14 @@
       <c r="H68" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I68" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Design, Direction and Creative Management</v>
-      </c>
-      <c r="J68" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Spencer Low</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I68" t="s">
+        <v>35</v>
+      </c>
+      <c r="J68" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69" s="4" t="s">
@@ -3079,16 +2963,14 @@
       <c r="H69" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I69" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Consumer Services</v>
-      </c>
-      <c r="J69" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I69" t="s">
+        <v>34</v>
+      </c>
+      <c r="J69" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70" s="3" t="s">
@@ -3106,16 +2988,14 @@
       <c r="H70" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I70" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Inbound Repair and Services</v>
-      </c>
-      <c r="J70" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I70" t="s">
+        <v>44</v>
+      </c>
+      <c r="J70" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71" s="4" t="s">
@@ -3133,16 +3013,14 @@
       <c r="H71" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I71" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Outbound Consumer Service</v>
-      </c>
-      <c r="J71" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jamie Reding</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I71" t="s">
+        <v>48</v>
+      </c>
+      <c r="J71" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72" s="3" t="s">
@@ -3160,16 +3038,14 @@
       <c r="H72" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I72" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Consulting</v>
-      </c>
-      <c r="J72" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Allie Bellew</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
+      <c r="J72" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73" s="4" t="s">
@@ -3187,16 +3063,14 @@
       <c r="H73" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="I73" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Distributors, Dispatchers and Processors</v>
-      </c>
-      <c r="J73" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Spencer Low</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I73" t="s">
+        <v>36</v>
+      </c>
+      <c r="J73" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74" s="3" t="s">
@@ -3214,16 +3088,14 @@
       <c r="H74" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I74" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Accounting</v>
-      </c>
-      <c r="J74" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Jamie Reding</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I74" t="s">
+        <v>28</v>
+      </c>
+      <c r="J74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75" s="4" t="s">
@@ -3241,16 +3113,14 @@
       <c r="H75" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I75" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Durable Manufacturing</v>
-      </c>
-      <c r="J75" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I75" t="s">
+        <v>38</v>
+      </c>
+      <c r="J75" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="3" t="s">
@@ -3268,16 +3138,14 @@
       <c r="H76" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I76" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Non-Durable Merchandise Retail</v>
-      </c>
-      <c r="J76" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Sanjay Shah</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I76" t="s">
+        <v>47</v>
+      </c>
+      <c r="J76" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="4" t="s">
@@ -3295,16 +3163,14 @@
       <c r="H77" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I77" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Insurance</v>
-      </c>
-      <c r="J77" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I77" t="s">
+        <v>45</v>
+      </c>
+      <c r="J77" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78" s="3" t="s">
@@ -3322,16 +3188,14 @@
       <c r="H78" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I78" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Building Supply Retail</v>
-      </c>
-      <c r="J78" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I78" t="s">
+        <v>32</v>
+      </c>
+      <c r="J78" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79" s="4" t="s">
@@ -3349,16 +3213,14 @@
       <c r="H79" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I79" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Insurance</v>
-      </c>
-      <c r="J79" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Molly Clark</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I79" t="s">
+        <v>45</v>
+      </c>
+      <c r="J79" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="3" t="s">
@@ -3376,16 +3238,14 @@
       <c r="H80" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I80" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Eating and Drinking Places</v>
-      </c>
-      <c r="J80" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Anne Weiler</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I80" t="s">
+        <v>39</v>
+      </c>
+      <c r="J80" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81" s="4" t="s">
@@ -3403,13 +3263,11 @@
       <c r="H81" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I81" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[IndustrySeq]],[1]!IndustryTbl[IndustrySeq],[1]!IndustryTbl[Industry])</f>
-        <v>Outbound Consumer Service</v>
-      </c>
-      <c r="J81" t="str">
-        <f>_xlfn.XLOOKUP([1]!AccountTbl[[#This Row],[AccountOwnerSeq]],[1]!OwnerTbl[SystemUserSeq],[1]!OwnerTbl[Owner],"")</f>
-        <v>Alicia Thomber</v>
+      <c r="I81" t="s">
+        <v>48</v>
+      </c>
+      <c r="J81" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3455,14 +3313,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>

</xml_diff>